<commit_message>
Done with download function, project more or less completed.
</commit_message>
<xml_diff>
--- a/full_year_2026_staff.xlsx
+++ b/full_year_2026_staff.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="112">
   <si>
     <t>Name</t>
   </si>
@@ -22,16 +22,16 @@
     <t>Role</t>
   </si>
   <si>
-    <t>Ytd_Points</t>
-  </si>
-  <si>
-    <t>Blackout_Dates</t>
-  </si>
-  <si>
-    <t>PH_Bidding</t>
-  </si>
-  <si>
-    <t>Last_PH_Worked</t>
+    <t>Ytd Points</t>
+  </si>
+  <si>
+    <t>Blackout Dates</t>
+  </si>
+  <si>
+    <t>PH Bidding</t>
+  </si>
+  <si>
+    <t>Last PH Worked</t>
   </si>
   <si>
     <t>PH Immunity Duration</t>
@@ -157,193 +157,196 @@
     <t>Nina Dobrev</t>
   </si>
   <si>
+    <t>NO_PM</t>
+  </si>
+  <si>
     <t>STANDARD</t>
   </si>
   <si>
-    <t>NO_PM</t>
-  </si>
-  <si>
     <t>WEEKEND_ONLY</t>
   </si>
   <si>
-    <t>2026-02-05, 2026-04-04, 2026-04-09, 2026-05-23, 2026-06-23, 2026-07-11, 2026-07-18, 2026-08-05, 2026-08-08, 2026-08-15, 2026-08-23, 2026-10-05, 2026-10-20, 2026-10-22, 2026-10-29, 2026-11-08, 2026-11-16, 2026-11-30, 2026-12-29</t>
-  </si>
-  <si>
-    <t>2026-01-07, 2026-02-07, 2026-02-21, 2026-03-07, 2026-04-05, 2026-04-08, 2026-05-06, 2026-05-13, 2026-05-30, 2026-06-09, 2026-06-17, 2026-07-13, 2026-08-30, 2026-09-15, 2026-10-27, 2026-11-01, 2026-11-02, 2026-11-12, 2026-12-11</t>
-  </si>
-  <si>
-    <t>2026-01-07, 2026-03-07, 2026-03-16, 2026-03-18, 2026-03-27, 2026-04-13, 2026-05-15, 2026-06-23, 2026-06-28, 2026-08-03, 2026-09-12, 2026-10-10, 2026-12-13, 2026-12-28</t>
-  </si>
-  <si>
-    <t>2026-01-02, 2026-01-11, 2026-01-17, 2026-02-08, 2026-04-20, 2026-04-21, 2026-06-12, 2026-08-04, 2026-08-17, 2026-08-18, 2026-08-26, 2026-09-14, 2026-09-18, 2026-11-14, 2026-12-22</t>
-  </si>
-  <si>
-    <t>2026-01-08, 2026-01-09, 2026-03-10, 2026-03-12, 2026-03-16, 2026-04-20, 2026-04-21, 2026-04-24, 2026-05-06, 2026-06-03, 2026-06-19, 2026-06-24, 2026-07-29, 2026-09-14, 2026-09-30, 2026-10-09, 2026-10-14, 2026-10-15, 2026-11-04, 2026-11-21, 2026-12-05, 2026-12-14, 2026-12-22</t>
-  </si>
-  <si>
-    <t>2026-01-22, 2026-03-01, 2026-03-05, 2026-03-29, 2026-04-05, 2026-04-10, 2026-04-16, 2026-04-20, 2026-04-28, 2026-06-12, 2026-06-27, 2026-07-11, 2026-07-21, 2026-07-25, 2026-07-31, 2026-08-28, 2026-09-26, 2026-10-29, 2026-12-05, 2026-12-07</t>
-  </si>
-  <si>
-    <t>2026-01-31, 2026-02-02, 2026-02-14, 2026-04-03, 2026-04-19, 2026-05-03, 2026-05-09, 2026-05-14, 2026-05-16, 2026-05-19, 2026-05-21, 2026-06-21, 2026-07-08, 2026-08-12, 2026-09-06, 2026-10-01, 2026-10-13, 2026-11-04, 2026-12-21, 2026-12-26</t>
-  </si>
-  <si>
-    <t>2026-03-21, 2026-05-02, 2026-05-11, 2026-05-27, 2026-06-24, 2026-07-12, 2026-07-13, 2026-07-16, 2026-09-30, 2026-10-19, 2026-10-23, 2026-11-02, 2026-11-14, 2026-11-30, 2026-12-02, 2026-12-08</t>
-  </si>
-  <si>
-    <t>2026-02-28, 2026-03-07, 2026-03-31, 2026-04-04, 2026-04-09, 2026-05-07, 2026-06-17, 2026-07-12, 2026-08-12, 2026-08-18, 2026-08-30, 2026-09-18, 2026-10-04, 2026-10-07, 2026-11-17, 2026-12-07, 2026-12-17, 2026-12-22, 2026-12-29</t>
-  </si>
-  <si>
-    <t>2026-01-04, 2026-01-12, 2026-02-03, 2026-02-16, 2026-02-25, 2026-03-08, 2026-03-14, 2026-03-25, 2026-04-08, 2026-05-12, 2026-05-26, 2026-05-28, 2026-05-30, 2026-06-16, 2026-08-05, 2026-08-18, 2026-12-04</t>
-  </si>
-  <si>
-    <t>2026-01-04, 2026-01-16, 2026-03-20, 2026-04-16, 2026-04-20, 2026-04-21, 2026-04-28, 2026-05-15, 2026-05-18, 2026-05-19, 2026-06-09, 2026-06-21, 2026-06-23, 2026-08-02, 2026-08-04, 2026-09-16, 2026-09-30, 2026-10-08, 2026-11-08, 2026-11-10, 2026-11-21, 2026-12-01, 2026-12-04, 2026-12-16</t>
-  </si>
-  <si>
-    <t>2026-01-02, 2026-01-12, 2026-01-20, 2026-02-16, 2026-02-21, 2026-03-16, 2026-04-06, 2026-04-13, 2026-05-13, 2026-05-16, 2026-05-17, 2026-05-25, 2026-07-06, 2026-08-29, 2026-09-05, 2026-09-14, 2026-09-21, 2026-10-10, 2026-11-08, 2026-11-09, 2026-12-14, 2026-12-26</t>
-  </si>
-  <si>
-    <t>2026-02-08, 2026-03-03, 2026-04-26, 2026-05-07, 2026-05-15, 2026-05-16, 2026-06-18, 2026-06-26, 2026-07-05, 2026-07-18, 2026-07-29, 2026-07-31, 2026-08-23, 2026-09-23, 2026-11-10, 2026-11-12, 2026-11-15, 2026-11-27</t>
-  </si>
-  <si>
-    <t>2026-01-20, 2026-01-31, 2026-02-21, 2026-03-04, 2026-03-10, 2026-03-24, 2026-05-23, 2026-05-25, 2026-06-08, 2026-06-13, 2026-08-14, 2026-09-06, 2026-10-07, 2026-12-06</t>
-  </si>
-  <si>
-    <t>2026-01-13, 2026-01-18, 2026-03-07, 2026-03-21, 2026-03-28, 2026-04-01, 2026-05-25, 2026-06-01, 2026-06-10, 2026-07-18, 2026-07-26, 2026-08-03, 2026-09-10, 2026-09-26, 2026-10-31, 2026-11-26, 2026-12-05</t>
-  </si>
-  <si>
-    <t>2026-01-06, 2026-01-12, 2026-01-21, 2026-02-05, 2026-02-21, 2026-03-10, 2026-03-14, 2026-05-21, 2026-06-17, 2026-06-18, 2026-08-11, 2026-08-26, 2026-09-17, 2026-09-25, 2026-11-11, 2026-11-29, 2026-12-07, 2026-12-13, 2026-12-20, 2026-12-21, 2026-12-26</t>
-  </si>
-  <si>
-    <t>2026-01-01, 2026-01-09, 2026-02-24, 2026-02-27, 2026-03-04, 2026-04-19, 2026-04-22, 2026-05-10, 2026-06-02, 2026-06-12, 2026-06-13, 2026-06-15, 2026-06-18, 2026-07-23, 2026-07-30, 2026-07-31, 2026-08-21, 2026-09-05, 2026-10-16, 2026-10-27, 2026-11-26, 2026-12-25</t>
-  </si>
-  <si>
-    <t>2026-01-08, 2026-01-24, 2026-01-26, 2026-01-31, 2026-02-03, 2026-03-12, 2026-03-18, 2026-03-23, 2026-05-11, 2026-05-13, 2026-05-15, 2026-06-03, 2026-06-15, 2026-06-21, 2026-06-26, 2026-06-30, 2026-07-15, 2026-08-11, 2026-08-12, 2026-09-01, 2026-09-19, 2026-10-20, 2026-10-29, 2026-11-26</t>
-  </si>
-  <si>
-    <t>2026-01-15, 2026-02-05, 2026-03-03, 2026-03-24, 2026-04-06, 2026-04-16, 2026-04-27, 2026-06-29, 2026-06-30, 2026-07-08, 2026-07-15, 2026-07-18, 2026-08-01, 2026-08-11, 2026-08-21, 2026-08-28, 2026-10-29, 2026-11-12, 2026-11-26, 2026-11-28</t>
-  </si>
-  <si>
-    <t>2026-01-08, 2026-01-12, 2026-01-26, 2026-01-28, 2026-03-04, 2026-03-22, 2026-03-25, 2026-03-30, 2026-04-03, 2026-04-04, 2026-04-16, 2026-04-26, 2026-05-01, 2026-05-14, 2026-05-15, 2026-05-28, 2026-07-04, 2026-07-21, 2026-08-15, 2026-08-22, 2026-09-14, 2026-12-12, 2026-12-13</t>
-  </si>
-  <si>
-    <t>2026-02-03, 2026-02-20, 2026-05-26, 2026-07-22, 2026-07-31, 2026-08-29, 2026-09-05, 2026-09-10, 2026-09-13, 2026-09-27, 2026-10-17, 2026-10-24, 2026-11-04, 2026-11-08, 2026-11-24</t>
-  </si>
-  <si>
-    <t>2026-01-01, 2026-01-09, 2026-02-06, 2026-02-27, 2026-03-23, 2026-04-12, 2026-05-17, 2026-05-26, 2026-06-01, 2026-06-10, 2026-06-22, 2026-07-14, 2026-08-04, 2026-08-17, 2026-08-20, 2026-09-19, 2026-09-26, 2026-12-12</t>
-  </si>
-  <si>
-    <t>2026-01-20, 2026-01-21, 2026-02-06, 2026-02-15, 2026-03-15, 2026-03-20, 2026-04-01, 2026-04-24, 2026-08-09, 2026-08-12, 2026-08-14, 2026-08-17, 2026-08-19, 2026-10-16, 2026-11-08, 2026-11-12, 2026-11-29, 2026-12-03, 2026-12-10</t>
-  </si>
-  <si>
-    <t>2026-01-20, 2026-02-17, 2026-05-21, 2026-05-25, 2026-06-02, 2026-06-07, 2026-07-12, 2026-08-08, 2026-08-24, 2026-09-03, 2026-09-23, 2026-09-24, 2026-09-26, 2026-11-27, 2026-12-03, 2026-12-15, 2026-12-28</t>
-  </si>
-  <si>
-    <t>2026-01-03, 2026-01-25, 2026-02-08, 2026-02-12, 2026-02-22, 2026-02-26, 2026-03-01, 2026-03-24, 2026-04-21, 2026-05-16, 2026-05-23, 2026-06-02, 2026-07-08, 2026-07-13, 2026-08-01, 2026-09-29, 2026-10-26, 2026-11-06, 2026-11-29, 2026-12-04, 2026-12-11, 2026-12-23, 2026-12-24</t>
-  </si>
-  <si>
-    <t>2026-01-10, 2026-01-16, 2026-01-31, 2026-02-04, 2026-02-16, 2026-02-17, 2026-02-27, 2026-03-13, 2026-03-30, 2026-04-26, 2026-05-19, 2026-07-17, 2026-08-11, 2026-08-15, 2026-08-17, 2026-09-10, 2026-10-01, 2026-10-09, 2026-11-08, 2026-11-10, 2026-11-13, 2026-11-16</t>
-  </si>
-  <si>
-    <t>2026-01-16, 2026-02-01, 2026-02-04, 2026-03-05, 2026-03-21, 2026-03-31, 2026-04-16, 2026-04-25, 2026-05-26, 2026-05-27, 2026-06-02, 2026-07-03, 2026-08-20, 2026-09-05, 2026-09-19, 2026-09-20, 2026-09-25, 2026-09-26, 2026-10-11, 2026-11-13, 2026-11-14, 2026-11-20, 2026-12-30</t>
-  </si>
-  <si>
-    <t>2026-04-15, 2026-05-14, 2026-05-16, 2026-06-03, 2026-06-18, 2026-07-22, 2026-07-31, 2026-08-02, 2026-08-16, 2026-08-17, 2026-08-31, 2026-09-15, 2026-12-05, 2026-12-12, 2026-12-28</t>
-  </si>
-  <si>
-    <t>2026-02-14, 2026-03-06, 2026-03-11, 2026-03-21, 2026-03-22, 2026-04-19, 2026-04-26, 2026-05-08, 2026-06-08, 2026-06-11, 2026-06-20, 2026-07-18, 2026-07-31, 2026-08-01, 2026-08-13, 2026-08-14, 2026-08-26, 2026-09-08, 2026-11-14, 2026-12-14, 2026-12-15, 2026-12-17</t>
-  </si>
-  <si>
-    <t>2026-01-16, 2026-01-22, 2026-01-23, 2026-01-26, 2026-01-27, 2026-03-12, 2026-03-22, 2026-04-09, 2026-05-26, 2026-09-07, 2026-09-10, 2026-10-04, 2026-10-13, 2026-10-23, 2026-11-21, 2026-11-24, 2026-11-27</t>
-  </si>
-  <si>
-    <t>2026-01-29, 2026-02-06, 2026-02-22, 2026-03-07, 2026-03-22, 2026-05-05, 2026-05-08, 2026-06-16, 2026-07-03, 2026-07-12, 2026-07-13, 2026-08-09, 2026-09-07, 2026-09-21, 2026-10-21, 2026-10-22, 2026-11-03, 2026-11-07, 2026-12-11, 2026-12-31</t>
-  </si>
-  <si>
-    <t>2026-01-30, 2026-02-08, 2026-02-26, 2026-03-09, 2026-05-10, 2026-06-18, 2026-06-30, 2026-07-05, 2026-08-03, 2026-08-16, 2026-08-26, 2026-09-08, 2026-09-26, 2026-10-01, 2026-11-03, 2026-11-08, 2026-12-18</t>
-  </si>
-  <si>
-    <t>2026-01-06, 2026-01-10, 2026-02-27, 2026-05-08, 2026-05-26, 2026-06-09, 2026-06-18, 2026-07-13, 2026-07-15, 2026-08-15, 2026-09-13, 2026-09-14, 2026-09-22, 2026-11-05, 2026-12-10</t>
-  </si>
-  <si>
-    <t>2026-02-10, 2026-02-16, 2026-03-14, 2026-03-15, 2026-04-04, 2026-04-05, 2026-04-12, 2026-04-21, 2026-04-29, 2026-05-23, 2026-06-02, 2026-06-16, 2026-06-29, 2026-08-11, 2026-09-25, 2026-10-07, 2026-10-28, 2026-11-02, 2026-12-01, 2026-12-17, 2026-12-20, 2026-12-24, 2026-12-26</t>
-  </si>
-  <si>
-    <t>2026-01-26, 2026-01-30, 2026-01-31, 2026-02-04, 2026-02-15, 2026-02-21, 2026-02-25, 2026-04-07, 2026-04-25, 2026-05-14, 2026-05-16, 2026-05-21, 2026-07-14, 2026-07-27, 2026-08-21, 2026-09-02, 2026-10-01, 2026-10-20, 2026-11-02, 2026-11-16, 2026-11-23, 2026-12-08, 2026-12-29</t>
-  </si>
-  <si>
-    <t>2026-01-11, 2026-01-21, 2026-01-30, 2026-02-07, 2026-02-21, 2026-03-18, 2026-04-23, 2026-05-03, 2026-05-21, 2026-07-05, 2026-07-16, 2026-07-26, 2026-08-26, 2026-10-03, 2026-10-31, 2026-11-01, 2026-11-14, 2026-11-26, 2026-12-31</t>
-  </si>
-  <si>
-    <t>2026-01-02, 2026-01-04, 2026-01-27, 2026-02-01, 2026-03-04, 2026-03-05, 2026-04-09, 2026-05-26, 2026-06-05, 2026-06-08, 2026-07-17, 2026-08-03, 2026-08-09, 2026-08-21, 2026-10-09, 2026-11-03, 2026-11-10, 2026-12-14, 2026-12-16, 2026-12-21, 2026-12-28</t>
-  </si>
-  <si>
-    <t>2026-01-20, 2026-02-16, 2026-03-15, 2026-04-28, 2026-05-25, 2026-06-01, 2026-06-09, 2026-06-24, 2026-07-15, 2026-07-29, 2026-08-16, 2026-08-20, 2026-08-27, 2026-08-28, 2026-10-08, 2026-10-22, 2026-11-09, 2026-11-11, 2026-11-16, 2026-11-18, 2026-12-17, 2026-12-31</t>
-  </si>
-  <si>
-    <t>2026-02-13, 2026-02-19, 2026-03-11, 2026-03-22, 2026-04-24, 2026-05-23, 2026-06-01, 2026-06-03, 2026-06-27, 2026-07-20, 2026-07-22, 2026-08-20, 2026-08-24, 2026-08-25, 2026-10-08, 2026-10-09, 2026-10-16, 2026-11-11, 2026-11-22, 2026-12-30</t>
-  </si>
-  <si>
-    <t>2026-01-13, 2026-01-18, 2026-01-28, 2026-02-02, 2026-02-22, 2026-03-29, 2026-04-15, 2026-04-25, 2026-05-23, 2026-06-07, 2026-06-26, 2026-07-17, 2026-08-01, 2026-08-12, 2026-08-14, 2026-08-26, 2026-08-28, 2026-10-10, 2026-10-12, 2026-12-11, 2026-12-29</t>
-  </si>
-  <si>
-    <t>2026-02-17, 2026-05-01, 2026-08-09</t>
-  </si>
-  <si>
-    <t>2026-05-21, 2026-08-09</t>
-  </si>
-  <si>
-    <t>2026-04-03, 2026-05-21</t>
-  </si>
-  <si>
-    <t>2026-04-03, 2026-12-25, 2026-06-03</t>
+    <t>2026-01-30, 2026-03-06, 2026-03-08, 2026-03-13, 2026-03-15, 2026-03-27, 2026-04-23, 2026-06-17, 2026-06-29, 2026-07-06, 2026-07-17, 2026-08-08, 2026-09-07, 2026-09-09, 2026-10-01, 2026-10-22, 2026-11-28, 2026-11-30, 2026-12-03</t>
+  </si>
+  <si>
+    <t>2026-01-17, 2026-02-11, 2026-02-27, 2026-04-19, 2026-05-27, 2026-05-29, 2026-06-02, 2026-07-25, 2026-07-30, 2026-09-18, 2026-09-27, 2026-10-08, 2026-10-12, 2026-10-21, 2026-10-30, 2026-11-08, 2026-11-10, 2026-11-14, 2026-11-21</t>
+  </si>
+  <si>
+    <t>2026-02-02, 2026-03-02, 2026-03-07, 2026-03-21, 2026-04-09, 2026-06-20, 2026-07-05, 2026-07-08, 2026-07-11, 2026-07-13, 2026-07-14, 2026-07-20, 2026-09-23, 2026-10-06, 2026-10-12</t>
+  </si>
+  <si>
+    <t>2026-01-06, 2026-02-03, 2026-03-07, 2026-04-06, 2026-04-14, 2026-04-18, 2026-05-04, 2026-07-14, 2026-08-07, 2026-08-22, 2026-08-23, 2026-09-29, 2026-10-29, 2026-11-02, 2026-12-12, 2026-12-17</t>
+  </si>
+  <si>
+    <t>2026-02-14, 2026-02-28, 2026-03-20, 2026-03-24, 2026-03-29, 2026-03-30, 2026-04-04, 2026-06-10, 2026-06-11, 2026-07-28, 2026-08-18, 2026-08-19, 2026-09-12, 2026-10-30, 2026-11-10, 2026-11-11, 2026-11-22, 2026-12-04, 2026-12-07, 2026-12-12, 2026-12-14, 2026-12-23, 2026-12-26</t>
+  </si>
+  <si>
+    <t>2026-01-08, 2026-01-29, 2026-02-10, 2026-02-17, 2026-03-08, 2026-03-17, 2026-03-19, 2026-03-30, 2026-05-03, 2026-05-25, 2026-06-05, 2026-08-15, 2026-09-08, 2026-10-30, 2026-12-29</t>
+  </si>
+  <si>
+    <t>2026-01-06, 2026-01-26, 2026-04-02, 2026-05-02, 2026-05-05, 2026-06-05, 2026-06-22, 2026-06-30, 2026-07-03, 2026-07-14, 2026-07-27, 2026-08-15, 2026-08-20, 2026-08-30, 2026-09-14, 2026-09-21, 2026-10-02, 2026-10-05</t>
+  </si>
+  <si>
+    <t>2026-02-02, 2026-02-18, 2026-02-20, 2026-03-14, 2026-03-26, 2026-05-27, 2026-07-24, 2026-07-31, 2026-08-28, 2026-10-16, 2026-10-20, 2026-11-02, 2026-11-20, 2026-11-27, 2026-12-21</t>
+  </si>
+  <si>
+    <t>2026-01-27, 2026-02-14, 2026-03-29, 2026-04-06, 2026-04-09, 2026-04-24, 2026-04-25, 2026-05-26, 2026-06-14, 2026-06-16, 2026-07-02, 2026-07-17, 2026-07-18, 2026-07-24, 2026-08-27, 2026-09-16, 2026-09-17, 2026-09-28, 2026-10-15, 2026-11-03, 2026-11-06, 2026-11-15, 2026-12-27</t>
+  </si>
+  <si>
+    <t>2026-01-12, 2026-01-23, 2026-02-18, 2026-02-23, 2026-03-30, 2026-05-25, 2026-06-27, 2026-07-06, 2026-07-07, 2026-08-20, 2026-08-21, 2026-09-03, 2026-09-04, 2026-09-19, 2026-09-28, 2026-10-23, 2026-11-10, 2026-11-25, 2026-11-27, 2026-12-16, 2026-12-31</t>
+  </si>
+  <si>
+    <t>2026-01-27, 2026-01-31, 2026-02-05, 2026-02-14, 2026-05-25, 2026-05-29, 2026-06-09, 2026-06-11, 2026-07-02, 2026-08-06, 2026-08-31, 2026-09-09, 2026-09-11, 2026-09-18, 2026-10-04, 2026-10-08, 2026-12-05, 2026-12-12</t>
+  </si>
+  <si>
+    <t>2026-01-11, 2026-03-11, 2026-04-03, 2026-04-05, 2026-04-06, 2026-04-17, 2026-04-29, 2026-05-25, 2026-06-01, 2026-06-25, 2026-07-05, 2026-07-29, 2026-08-11, 2026-09-29, 2026-10-26, 2026-10-29, 2026-10-31, 2026-11-11, 2026-12-06, 2026-12-08, 2026-12-22, 2026-12-24</t>
+  </si>
+  <si>
+    <t>2026-01-14, 2026-01-16, 2026-01-28, 2026-03-04, 2026-03-09, 2026-05-28, 2026-06-09, 2026-06-27, 2026-07-18, 2026-07-31, 2026-08-01, 2026-08-14, 2026-08-17, 2026-08-27, 2026-09-04, 2026-10-10, 2026-11-24, 2026-12-03, 2026-12-05, 2026-12-13, 2026-12-27</t>
+  </si>
+  <si>
+    <t>2026-01-26, 2026-01-27, 2026-02-03, 2026-02-13, 2026-02-22, 2026-03-07, 2026-03-14, 2026-04-10, 2026-07-22, 2026-08-02, 2026-08-10, 2026-08-15, 2026-08-18, 2026-08-27, 2026-09-24, 2026-11-07, 2026-12-04, 2026-12-29</t>
+  </si>
+  <si>
+    <t>2026-01-08, 2026-01-19, 2026-01-24, 2026-01-29, 2026-03-09, 2026-03-31, 2026-04-14, 2026-04-27, 2026-05-01, 2026-05-04, 2026-06-29, 2026-07-03, 2026-09-16, 2026-09-25, 2026-09-26, 2026-10-21, 2026-10-24, 2026-10-31, 2026-11-04, 2026-11-16, 2026-12-09, 2026-12-10, 2026-12-11, 2026-12-24</t>
+  </si>
+  <si>
+    <t>2026-01-06, 2026-01-09, 2026-01-16, 2026-01-30, 2026-02-03, 2026-02-21, 2026-02-24, 2026-04-03, 2026-04-17, 2026-05-01, 2026-06-19, 2026-08-09, 2026-08-12, 2026-09-16, 2026-09-17, 2026-10-02, 2026-10-21, 2026-10-25, 2026-11-12, 2026-11-28, 2026-11-29, 2026-12-19</t>
+  </si>
+  <si>
+    <t>2026-01-02, 2026-01-27, 2026-02-10, 2026-02-12, 2026-02-20, 2026-02-23, 2026-02-24, 2026-03-27, 2026-05-05, 2026-05-10, 2026-06-01, 2026-06-14, 2026-08-08, 2026-08-19, 2026-09-08, 2026-11-13, 2026-12-18, 2026-12-19</t>
+  </si>
+  <si>
+    <t>2026-01-27, 2026-02-25, 2026-03-22, 2026-03-30, 2026-05-06, 2026-05-08, 2026-05-11, 2026-06-05, 2026-06-18, 2026-07-07, 2026-07-20, 2026-07-25, 2026-08-04, 2026-08-17, 2026-10-01, 2026-11-10, 2026-12-02, 2026-12-19</t>
+  </si>
+  <si>
+    <t>2026-01-27, 2026-03-03, 2026-03-12, 2026-05-11, 2026-06-09, 2026-06-21, 2026-07-05, 2026-07-16, 2026-07-28, 2026-09-09, 2026-09-21, 2026-10-02, 2026-10-10, 2026-11-06, 2026-11-18</t>
+  </si>
+  <si>
+    <t>2026-01-07, 2026-01-21, 2026-01-29, 2026-01-30, 2026-02-17, 2026-06-01, 2026-06-23, 2026-06-29, 2026-08-17, 2026-09-11, 2026-09-20, 2026-11-15, 2026-11-25, 2026-11-27, 2026-12-24</t>
+  </si>
+  <si>
+    <t>2026-01-30, 2026-02-26, 2026-03-09, 2026-04-13, 2026-04-19, 2026-04-27, 2026-05-05, 2026-05-25, 2026-06-04, 2026-07-02, 2026-07-08, 2026-07-27, 2026-08-04, 2026-08-25, 2026-09-16, 2026-10-20, 2026-12-01, 2026-12-07</t>
+  </si>
+  <si>
+    <t>2026-01-02, 2026-01-03, 2026-02-21, 2026-02-23, 2026-02-25, 2026-02-26, 2026-03-13, 2026-03-14, 2026-04-09, 2026-05-30, 2026-06-20, 2026-06-27, 2026-07-22, 2026-08-04, 2026-08-06, 2026-08-29, 2026-09-16, 2026-10-22, 2026-11-26, 2026-11-27, 2026-12-15, 2026-12-29</t>
+  </si>
+  <si>
+    <t>2026-02-19, 2026-03-17, 2026-03-28, 2026-05-10, 2026-05-16, 2026-06-30, 2026-08-10, 2026-08-18, 2026-08-20, 2026-09-03, 2026-09-13, 2026-11-05, 2026-11-20, 2026-11-22, 2026-11-28</t>
+  </si>
+  <si>
+    <t>2026-01-04, 2026-02-05, 2026-02-23, 2026-03-20, 2026-04-08, 2026-04-09, 2026-04-17, 2026-05-01, 2026-05-05, 2026-05-10, 2026-06-22, 2026-06-27, 2026-07-18, 2026-07-28, 2026-08-08, 2026-08-10, 2026-08-27, 2026-10-09, 2026-12-12, 2026-12-29</t>
+  </si>
+  <si>
+    <t>2026-01-09, 2026-01-11, 2026-01-19, 2026-02-21, 2026-03-27, 2026-04-04, 2026-05-06, 2026-07-15, 2026-07-22, 2026-07-23, 2026-08-06, 2026-09-16, 2026-09-26, 2026-10-22, 2026-10-30, 2026-12-30</t>
+  </si>
+  <si>
+    <t>2026-03-06, 2026-03-27, 2026-04-02, 2026-05-21, 2026-06-05, 2026-07-02, 2026-07-09, 2026-08-15, 2026-08-18, 2026-09-14, 2026-10-09, 2026-10-13, 2026-12-08, 2026-12-10, 2026-12-19</t>
+  </si>
+  <si>
+    <t>2026-02-23, 2026-03-13, 2026-03-18, 2026-03-22, 2026-03-23, 2026-03-25, 2026-05-04, 2026-05-15, 2026-05-27, 2026-06-19, 2026-08-06, 2026-09-22, 2026-09-27, 2026-10-07, 2026-11-07, 2026-11-19, 2026-11-30</t>
+  </si>
+  <si>
+    <t>2026-01-06, 2026-01-08, 2026-01-14, 2026-01-17, 2026-01-23, 2026-02-05, 2026-02-16, 2026-02-23, 2026-03-02, 2026-03-28, 2026-04-05, 2026-04-07, 2026-04-18, 2026-04-28, 2026-09-09, 2026-09-15, 2026-09-25, 2026-10-11, 2026-10-14, 2026-10-24, 2026-11-29, 2026-12-06, 2026-12-09, 2026-12-21</t>
+  </si>
+  <si>
+    <t>2026-01-14, 2026-02-08, 2026-02-10, 2026-03-02, 2026-03-11, 2026-03-14, 2026-03-16, 2026-03-18, 2026-04-18, 2026-04-29, 2026-06-10, 2026-06-22, 2026-06-24, 2026-06-28, 2026-07-20, 2026-07-24, 2026-11-10, 2026-12-05, 2026-12-06, 2026-12-11, 2026-12-22</t>
+  </si>
+  <si>
+    <t>2026-01-23, 2026-01-31, 2026-02-08, 2026-02-23, 2026-02-26, 2026-03-18, 2026-07-03, 2026-07-13, 2026-07-28, 2026-08-04, 2026-09-02, 2026-11-01, 2026-11-07, 2026-11-16, 2026-12-23, 2026-12-25</t>
+  </si>
+  <si>
+    <t>2026-01-10, 2026-01-17, 2026-02-11, 2026-02-20, 2026-03-26, 2026-03-31, 2026-04-21, 2026-05-03, 2026-05-20, 2026-05-28, 2026-05-30, 2026-06-12, 2026-06-19, 2026-09-06, 2026-09-25, 2026-10-23, 2026-12-03</t>
+  </si>
+  <si>
+    <t>2026-01-03, 2026-01-30, 2026-01-31, 2026-02-25, 2026-04-10, 2026-04-18, 2026-05-14, 2026-05-15, 2026-06-07, 2026-06-14, 2026-06-15, 2026-08-10, 2026-09-01, 2026-09-21, 2026-10-25, 2026-11-03, 2026-11-21, 2026-12-07</t>
+  </si>
+  <si>
+    <t>2026-01-05, 2026-02-08, 2026-02-25, 2026-03-07, 2026-03-30, 2026-04-04, 2026-04-24, 2026-05-21, 2026-05-28, 2026-06-10, 2026-06-15, 2026-06-17, 2026-07-20, 2026-07-25, 2026-07-26, 2026-08-03, 2026-08-10, 2026-09-15, 2026-10-02, 2026-11-20, 2026-11-24, 2026-11-30, 2026-12-02, 2026-12-07</t>
+  </si>
+  <si>
+    <t>2026-01-01, 2026-01-14, 2026-03-07, 2026-03-10, 2026-03-22, 2026-04-25, 2026-05-10, 2026-05-11, 2026-08-07, 2026-08-21, 2026-09-25, 2026-10-18, 2026-10-29, 2026-11-04, 2026-11-07, 2026-11-19, 2026-11-21, 2026-12-26</t>
+  </si>
+  <si>
+    <t>2026-01-15, 2026-03-16, 2026-04-09, 2026-04-14, 2026-04-22, 2026-05-17, 2026-06-21, 2026-06-28, 2026-07-05, 2026-07-11, 2026-07-31, 2026-08-31, 2026-09-02, 2026-09-05, 2026-09-14, 2026-09-24, 2026-10-25, 2026-11-13, 2026-11-24, 2026-11-25</t>
+  </si>
+  <si>
+    <t>2026-01-05, 2026-02-05, 2026-02-22, 2026-03-01, 2026-03-11, 2026-03-14, 2026-03-19, 2026-04-18, 2026-08-03, 2026-08-10, 2026-08-13, 2026-08-19, 2026-08-23, 2026-09-24, 2026-10-09, 2026-10-10, 2026-10-20, 2026-11-16, 2026-11-25, 2026-12-09, 2026-12-17, 2026-12-25</t>
+  </si>
+  <si>
+    <t>2026-01-12, 2026-02-10, 2026-02-25, 2026-03-05, 2026-03-09, 2026-03-10, 2026-03-13, 2026-04-04, 2026-04-15, 2026-05-13, 2026-05-14, 2026-06-02, 2026-06-11, 2026-06-19, 2026-07-15, 2026-07-19, 2026-08-23, 2026-09-09, 2026-09-27, 2026-09-28, 2026-09-30, 2026-10-09, 2026-11-28, 2026-12-04</t>
+  </si>
+  <si>
+    <t>2026-03-09, 2026-03-20, 2026-04-11, 2026-04-13, 2026-04-27, 2026-05-01, 2026-05-10, 2026-05-11, 2026-06-13, 2026-06-27, 2026-06-29, 2026-08-27, 2026-11-05, 2026-12-14, 2026-12-28</t>
+  </si>
+  <si>
+    <t>2026-01-07, 2026-01-19, 2026-01-22, 2026-01-31, 2026-03-03, 2026-03-15, 2026-03-19, 2026-03-24, 2026-03-27, 2026-05-28, 2026-06-09, 2026-06-10, 2026-06-14, 2026-06-26, 2026-06-29, 2026-07-14, 2026-07-31, 2026-08-20, 2026-08-30, 2026-10-23, 2026-10-29, 2026-12-18, 2026-12-23</t>
+  </si>
+  <si>
+    <t>2026-01-02, 2026-01-08, 2026-01-17, 2026-01-28, 2026-02-13, 2026-02-19, 2026-02-27, 2026-02-28, 2026-03-14, 2026-04-08, 2026-04-17, 2026-06-01, 2026-06-03, 2026-08-23, 2026-08-30, 2026-09-14, 2026-10-28, 2026-11-04, 2026-11-08, 2026-11-10, 2026-12-01, 2026-12-28</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>2026-05-01, 2026-08-09</t>
-  </si>
-  <si>
-    <t>2026-02-18, 2026-02-17, 2026-04-03</t>
+    <t>2026-02-18, 2026-05-01, 2026-08-09</t>
+  </si>
+  <si>
+    <t>2026-12-25, 2026-06-03</t>
+  </si>
+  <si>
+    <t>2026-12-25, 2026-02-18</t>
+  </si>
+  <si>
+    <t>2026-12-25, 2026-05-01, 2026-02-18</t>
+  </si>
+  <si>
+    <t>2026-12-25, 2026-02-17, 2026-08-09</t>
   </si>
   <si>
     <t>2026-02-18</t>
   </si>
   <si>
+    <t>2026-12-25, 2026-04-03, 2026-05-01</t>
+  </si>
+  <si>
+    <t>2026-02-17</t>
+  </si>
+  <si>
+    <t>2026-02-17, 2026-12-25</t>
+  </si>
+  <si>
+    <t>2026-02-17, 2026-04-03</t>
+  </si>
+  <si>
+    <t>2026-05-01, 2026-06-03, 2026-08-09</t>
+  </si>
+  <si>
+    <t>2026-02-18, 2026-04-03, 2026-12-25</t>
+  </si>
+  <si>
+    <t>2026-05-21, 2026-12-25</t>
+  </si>
+  <si>
+    <t>2026-02-17, 2026-02-18</t>
+  </si>
+  <si>
+    <t>2026-02-18, 2026-05-01, 2026-05-21</t>
+  </si>
+  <si>
+    <t>2026-05-01, 2026-02-18</t>
+  </si>
+  <si>
+    <t>2026-05-01, 2026-05-21</t>
+  </si>
+  <si>
+    <t>2026-02-17, 2026-08-09</t>
+  </si>
+  <si>
     <t>2026-12-25</t>
   </si>
   <si>
-    <t>2026-04-03, 2026-05-01, 2026-02-18</t>
-  </si>
-  <si>
-    <t>2026-08-09, 2026-05-01</t>
-  </si>
-  <si>
-    <t>2026-02-18, 2026-04-03</t>
-  </si>
-  <si>
-    <t>2026-06-03, 2026-04-03</t>
-  </si>
-  <si>
-    <t>2026-06-03, 2026-02-17, 2026-05-21</t>
-  </si>
-  <si>
-    <t>2026-05-01</t>
-  </si>
-  <si>
-    <t>2026-06-03, 2026-08-09, 2026-05-21</t>
-  </si>
-  <si>
-    <t>2026-12-25, 2026-05-01, 2026-04-03</t>
-  </si>
-  <si>
-    <t>2026-02-17</t>
-  </si>
-  <si>
-    <t>2026-04-03, 2026-02-18</t>
-  </si>
-  <si>
-    <t>2026-05-21, 2026-08-09, 2026-02-18</t>
+    <t>2026-05-21</t>
   </si>
   <si>
     <t>2026-01-18 - 2026-04-28</t>
@@ -752,7 +755,7 @@
         <v>47</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>50</v>
@@ -760,11 +763,11 @@
       <c r="E2" t="s">
         <v>90</v>
       </c>
-      <c r="F2" t="s">
-        <v>94</v>
+      <c r="F2" s="2">
+        <v>46040</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -772,22 +775,22 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C3">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
         <v>51</v>
       </c>
       <c r="E3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F3" s="2">
         <v>46040</v>
       </c>
       <c r="G3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -798,19 +801,19 @@
         <v>47</v>
       </c>
       <c r="C4">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>52</v>
       </c>
       <c r="E4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -818,22 +821,22 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C5">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
         <v>53</v>
       </c>
       <c r="E5" t="s">
-        <v>93</v>
-      </c>
-      <c r="F5" s="2">
-        <v>46040</v>
+        <v>90</v>
+      </c>
+      <c r="F5" t="s">
+        <v>90</v>
       </c>
       <c r="G5" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -841,22 +844,22 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
         <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>94</v>
-      </c>
-      <c r="F6" t="s">
-        <v>94</v>
+        <v>90</v>
+      </c>
+      <c r="F6" s="2">
+        <v>46040</v>
       </c>
       <c r="G6" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -867,19 +870,19 @@
         <v>47</v>
       </c>
       <c r="C7">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
         <v>55</v>
       </c>
       <c r="E7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F7" s="2">
         <v>46040</v>
       </c>
       <c r="G7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -890,19 +893,19 @@
         <v>47</v>
       </c>
       <c r="C8">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>56</v>
       </c>
       <c r="E8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F8" s="2">
         <v>46040</v>
       </c>
       <c r="G8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -913,19 +916,19 @@
         <v>47</v>
       </c>
       <c r="C9">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
         <v>57</v>
       </c>
       <c r="E9" t="s">
-        <v>95</v>
-      </c>
-      <c r="F9" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+      <c r="F9" s="2">
+        <v>46040</v>
       </c>
       <c r="G9" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -936,19 +939,19 @@
         <v>48</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
         <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>94</v>
-      </c>
-      <c r="F10" s="2">
-        <v>46040</v>
+        <v>90</v>
+      </c>
+      <c r="F10" t="s">
+        <v>90</v>
       </c>
       <c r="G10" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -959,19 +962,19 @@
         <v>48</v>
       </c>
       <c r="C11">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
         <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>94</v>
-      </c>
-      <c r="F11" s="2">
-        <v>46040</v>
+        <v>90</v>
+      </c>
+      <c r="F11" t="s">
+        <v>90</v>
       </c>
       <c r="G11" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -979,22 +982,22 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C12">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
         <v>60</v>
       </c>
       <c r="E12" t="s">
-        <v>96</v>
-      </c>
-      <c r="F12" t="s">
         <v>94</v>
       </c>
+      <c r="F12" s="2">
+        <v>46040</v>
+      </c>
       <c r="G12" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1002,7 +1005,7 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C13">
         <v>14</v>
@@ -1011,13 +1014,13 @@
         <v>61</v>
       </c>
       <c r="E13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F13" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G13" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1025,22 +1028,22 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C14">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D14" t="s">
         <v>62</v>
       </c>
       <c r="E14" t="s">
-        <v>98</v>
-      </c>
-      <c r="F14" t="s">
-        <v>94</v>
+        <v>96</v>
+      </c>
+      <c r="F14" s="2">
+        <v>46040</v>
       </c>
       <c r="G14" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1048,22 +1051,22 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
         <v>63</v>
       </c>
       <c r="E15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F15" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G15" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1071,22 +1074,22 @@
         <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C16">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s">
         <v>64</v>
       </c>
       <c r="E16" t="s">
-        <v>100</v>
-      </c>
-      <c r="F16" s="2">
-        <v>46040</v>
+        <v>90</v>
+      </c>
+      <c r="F16" t="s">
+        <v>90</v>
       </c>
       <c r="G16" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1094,22 +1097,22 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C17">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D17" t="s">
         <v>65</v>
       </c>
       <c r="E17" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="F17" s="2">
         <v>46040</v>
       </c>
       <c r="G17" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1117,22 +1120,22 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D18" t="s">
         <v>66</v>
       </c>
       <c r="E18" t="s">
-        <v>94</v>
-      </c>
-      <c r="F18" t="s">
-        <v>94</v>
+        <v>90</v>
+      </c>
+      <c r="F18" s="2">
+        <v>46040</v>
       </c>
       <c r="G18" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1140,22 +1143,22 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s">
         <v>67</v>
       </c>
       <c r="E19" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="F19" s="2">
         <v>46040</v>
       </c>
       <c r="G19" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1163,22 +1166,22 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C20">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D20" t="s">
         <v>68</v>
       </c>
       <c r="E20" t="s">
-        <v>94</v>
-      </c>
-      <c r="F20" s="2">
-        <v>46040</v>
+        <v>100</v>
+      </c>
+      <c r="F20" t="s">
+        <v>90</v>
       </c>
       <c r="G20" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1186,22 +1189,22 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C21">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D21" t="s">
         <v>69</v>
       </c>
       <c r="E21" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F21" s="2">
         <v>46040</v>
       </c>
       <c r="G21" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1209,22 +1212,22 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C22">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D22" t="s">
         <v>70</v>
       </c>
       <c r="E22" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F22" s="2">
         <v>46040</v>
       </c>
       <c r="G22" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1232,22 +1235,22 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C23">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D23" t="s">
         <v>71</v>
       </c>
       <c r="E23" t="s">
-        <v>102</v>
-      </c>
-      <c r="F23" t="s">
-        <v>94</v>
+        <v>90</v>
+      </c>
+      <c r="F23" s="2">
+        <v>46040</v>
       </c>
       <c r="G23" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1255,22 +1258,22 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C24">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D24" t="s">
         <v>72</v>
       </c>
       <c r="E24" t="s">
-        <v>94</v>
-      </c>
-      <c r="F24" s="2">
-        <v>46040</v>
+        <v>90</v>
+      </c>
+      <c r="F24" t="s">
+        <v>90</v>
       </c>
       <c r="G24" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1281,19 +1284,19 @@
         <v>47</v>
       </c>
       <c r="C25">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D25" t="s">
         <v>73</v>
       </c>
       <c r="E25" t="s">
-        <v>94</v>
-      </c>
-      <c r="F25" t="s">
-        <v>94</v>
+        <v>90</v>
+      </c>
+      <c r="F25" s="2">
+        <v>46040</v>
       </c>
       <c r="G25" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1301,22 +1304,22 @@
         <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C26">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D26" t="s">
         <v>74</v>
       </c>
       <c r="E26" t="s">
-        <v>103</v>
-      </c>
-      <c r="F26" s="2">
-        <v>46040</v>
+        <v>102</v>
+      </c>
+      <c r="F26" t="s">
+        <v>90</v>
       </c>
       <c r="G26" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1324,22 +1327,22 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C27">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D27" t="s">
         <v>75</v>
       </c>
       <c r="E27" t="s">
-        <v>94</v>
-      </c>
-      <c r="F27" s="2">
-        <v>46040</v>
+        <v>103</v>
+      </c>
+      <c r="F27" t="s">
+        <v>90</v>
       </c>
       <c r="G27" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1347,10 +1350,10 @@
         <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C28">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D28" t="s">
         <v>76</v>
@@ -1359,10 +1362,10 @@
         <v>104</v>
       </c>
       <c r="F28" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G28" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1370,10 +1373,10 @@
         <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C29">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D29" t="s">
         <v>77</v>
@@ -1381,11 +1384,11 @@
       <c r="E29" t="s">
         <v>105</v>
       </c>
-      <c r="F29" t="s">
-        <v>94</v>
+      <c r="F29" s="2">
+        <v>46040</v>
       </c>
       <c r="G29" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1393,22 +1396,22 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C30">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D30" t="s">
         <v>78</v>
       </c>
       <c r="E30" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="F30" s="2">
         <v>46040</v>
       </c>
       <c r="G30" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1416,22 +1419,22 @@
         <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C31">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D31" t="s">
         <v>79</v>
       </c>
       <c r="E31" t="s">
-        <v>94</v>
-      </c>
-      <c r="F31" s="2">
-        <v>46040</v>
+        <v>90</v>
+      </c>
+      <c r="F31" t="s">
+        <v>90</v>
       </c>
       <c r="G31" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1439,22 +1442,22 @@
         <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C32">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D32" t="s">
         <v>80</v>
       </c>
       <c r="E32" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="F32" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G32" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1462,22 +1465,22 @@
         <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C33">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D33" t="s">
         <v>81</v>
       </c>
       <c r="E33" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F33" s="2">
         <v>46040</v>
       </c>
       <c r="G33" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1485,22 +1488,22 @@
         <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D34" t="s">
         <v>82</v>
       </c>
       <c r="E34" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F34" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G34" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1508,22 +1511,22 @@
         <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C35">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D35" t="s">
         <v>83</v>
       </c>
       <c r="E35" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="F35" s="2">
         <v>46040</v>
       </c>
       <c r="G35" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1534,19 +1537,19 @@
         <v>47</v>
       </c>
       <c r="C36">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D36" t="s">
         <v>84</v>
       </c>
       <c r="E36" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="F36" s="2">
         <v>46040</v>
       </c>
       <c r="G36" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1554,22 +1557,22 @@
         <v>42</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C37">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D37" t="s">
         <v>85</v>
       </c>
       <c r="E37" t="s">
-        <v>97</v>
-      </c>
-      <c r="F37" t="s">
-        <v>94</v>
+        <v>90</v>
+      </c>
+      <c r="F37" s="2">
+        <v>46040</v>
       </c>
       <c r="G37" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1577,22 +1580,22 @@
         <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C38">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D38" t="s">
         <v>86</v>
       </c>
       <c r="E38" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="F38" s="2">
         <v>46040</v>
       </c>
       <c r="G38" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1600,22 +1603,22 @@
         <v>44</v>
       </c>
       <c r="B39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C39">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D39" t="s">
         <v>87</v>
       </c>
       <c r="E39" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="F39" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G39" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1623,22 +1626,22 @@
         <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C40">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D40" t="s">
         <v>88</v>
       </c>
       <c r="E40" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="F40" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G40" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1646,22 +1649,22 @@
         <v>46</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C41">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D41" t="s">
         <v>89</v>
       </c>
       <c r="E41" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="F41" s="2">
         <v>46040</v>
       </c>
       <c r="G41" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>